<commit_message>
Atualizando o site e o product backlog
</commit_message>
<xml_diff>
--- a/TI/produck-backlog.xlsx
+++ b/TI/produck-backlog.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\WINDOWS\Desktop\projeto-individual\TI\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4B45A4B-B21E-46FD-BF41-19E3FC2BF69D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A550C444-2945-46E7-AE50-4AD9B39D022F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{67496DB9-1C12-4816-A382-459BEB283ECC}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="50">
   <si>
     <t>Product Backlog</t>
   </si>
@@ -116,6 +116,87 @@
   </si>
   <si>
     <t>PP</t>
+  </si>
+  <si>
+    <t>tela de forum</t>
+  </si>
+  <si>
+    <t>funcional</t>
+  </si>
+  <si>
+    <t>desejavel</t>
+  </si>
+  <si>
+    <t>SPRINT 1</t>
+  </si>
+  <si>
+    <t>SPRINT 2</t>
+  </si>
+  <si>
+    <t>SPRINT 3</t>
+  </si>
+  <si>
+    <t>SPRINT 4</t>
+  </si>
+  <si>
+    <t>Tela incicial onde será a
+a primeira tela que o usuario 
+vai visualizar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tela de login onde o usário 
+vai acessar sua conta </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tela de perfil onde
+o usuario poderá ver seus 
+dados, desempenhos, entre
+outras coisas. </t>
+  </si>
+  <si>
+    <t>Tela de cadastro
+onde o usuario fará o cadastro
+para adquirir uma 
+conta na plataforma</t>
+  </si>
+  <si>
+    <t>Tela de sobre onde
+terá informações sobre
+a empresa</t>
+  </si>
+  <si>
+    <t>Tela de quis aonde o 
+usuario respondera algumas perguntas 
+para testar seu conhecimento</t>
+  </si>
+  <si>
+    <t>Formalização do projeto 
+garantindo a sua continuidade.</t>
+  </si>
+  <si>
+    <t>Criação das entidades e inserção 
+de dados.</t>
+  </si>
+  <si>
+    <t>Relacionamento entre as
+ entidades.</t>
+  </si>
+  <si>
+    <t>Ferramenta de gestão de
+projetos</t>
+  </si>
+  <si>
+    <t>Indicação e classificação
+ dos analytics.</t>
+  </si>
+  <si>
+    <t>Criação do repositorio
+no github</t>
+  </si>
+  <si>
+    <t>Tela de forum onde
+os usuários do site
+poderam interagir entre si</t>
   </si>
 </sst>
 </file>
@@ -202,7 +283,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -218,7 +299,10 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -534,10 +618,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E0B76C4D-D953-4D8E-BEA3-2245CE848EF8}">
-  <dimension ref="A1:J14"/>
+  <dimension ref="A1:J15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -592,172 +676,316 @@
       </c>
       <c r="I2" s="2"/>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+    <row r="3" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+      <c r="A3" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="C3" t="s">
+      <c r="B3" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="C3" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" s="6" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="F3" s="6"/>
+      <c r="G3" s="6">
+        <v>5</v>
+      </c>
+      <c r="H3" s="6" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="C4" t="s">
+      <c r="B4" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="C4" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E4" s="6" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="F4" s="6"/>
+      <c r="G4" s="6">
+        <v>2</v>
+      </c>
+      <c r="H4" s="6" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="75" x14ac:dyDescent="0.25">
+      <c r="A5" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="C5" t="s">
+      <c r="B5" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="C5" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="E5" t="s">
+      <c r="E5" s="6" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="F5" s="6"/>
+      <c r="G5" s="6">
+        <v>1</v>
+      </c>
+      <c r="H5" s="6" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" ht="75" x14ac:dyDescent="0.25">
+      <c r="A6" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C6" t="s">
+      <c r="B6" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="C6" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="E6" t="s">
+      <c r="E6" s="6" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="F6" s="6"/>
+      <c r="G6" s="6">
+        <v>6</v>
+      </c>
+      <c r="H6" s="6" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="A7" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="C7" t="s">
+      <c r="B7" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="C7" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D7" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="E7" t="s">
+      <c r="E7" s="6" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+      <c r="F7" s="6"/>
+      <c r="G7" s="6">
+        <v>7</v>
+      </c>
+      <c r="H7" s="6" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" ht="75" x14ac:dyDescent="0.25">
+      <c r="A8" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="C8" t="s">
+      <c r="B8" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="C8" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D8" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="E8" t="s">
+      <c r="E8" s="6" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+      <c r="F8" s="6"/>
+      <c r="G8" s="6">
+        <v>8</v>
+      </c>
+      <c r="H8" s="6" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="A9" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="C9" t="s">
+      <c r="B9" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="C9" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D9" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="E9" t="s">
+      <c r="E9" s="6" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+      <c r="F9" s="6"/>
+      <c r="G9" s="6">
+        <v>3</v>
+      </c>
+      <c r="H9" s="6" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="A10" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="C10" t="s">
+      <c r="B10" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="C10" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="D10" t="s">
+      <c r="D10" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="E10" t="s">
+      <c r="E10" s="6" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+      <c r="F10" s="6"/>
+      <c r="G10" s="6">
+        <v>9</v>
+      </c>
+      <c r="H10" s="6" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A11" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="C11" t="s">
+      <c r="B11" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="C11" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="D11" t="s">
+      <c r="D11" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="E11" t="s">
+      <c r="E11" s="6" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+      <c r="F11" s="6"/>
+      <c r="G11" s="6">
+        <v>10</v>
+      </c>
+      <c r="H11" s="6" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A12" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="C12" t="s">
+      <c r="B12" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="C12" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="D12" t="s">
+      <c r="D12" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="E12" t="s">
+      <c r="E12" s="6" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+      <c r="F12" s="6"/>
+      <c r="G12" s="6">
+        <v>4</v>
+      </c>
+      <c r="H12" s="6" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A13" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="C13" t="s">
+      <c r="B13" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="C13" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="D13" t="s">
+      <c r="D13" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="E13" t="s">
+      <c r="E13" s="6" t="s">
         <v>27</v>
       </c>
+      <c r="F13" s="6"/>
+      <c r="G13" s="6">
+        <v>12</v>
+      </c>
+      <c r="H13" s="6" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="14" spans="1:10" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="6" t="s">
+      <c r="A14" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="C14" t="s">
+      <c r="B14" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="C14" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="D14" t="s">
+      <c r="D14" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="E14" t="s">
+      <c r="E14" s="6" t="s">
         <v>29</v>
+      </c>
+      <c r="F14" s="6"/>
+      <c r="G14" s="6">
+        <v>5</v>
+      </c>
+      <c r="H14" s="6" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="A15" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="B15" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="C15" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="D15" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="E15" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="F15" s="6"/>
+      <c r="G15" s="6">
+        <v>11</v>
+      </c>
+      <c r="H15" s="6" t="s">
+        <v>35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Parte final do projeto
</commit_message>
<xml_diff>
--- a/TI/produck-backlog.xlsx
+++ b/TI/produck-backlog.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\WINDOWS\Desktop\projeto-individual\TI\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\WINDOWS\Desktop\aula\projeto-individual\TI\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A550C444-2945-46E7-AE50-4AD9B39D022F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF555C3F-6EB9-4F57-A600-4651419B2D72}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{67496DB9-1C12-4816-A382-459BEB283ECC}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="53">
   <si>
     <t>Product Backlog</t>
   </si>
@@ -67,9 +67,6 @@
   </si>
   <si>
     <t>Tela sobre</t>
-  </si>
-  <si>
-    <t>Tela do quis</t>
   </si>
   <si>
     <t>documentação</t>
@@ -116,15 +113,6 @@
   </si>
   <si>
     <t>PP</t>
-  </si>
-  <si>
-    <t>tela de forum</t>
-  </si>
-  <si>
-    <t>funcional</t>
-  </si>
-  <si>
-    <t>desejavel</t>
   </si>
   <si>
     <t>SPRINT 1</t>
@@ -194,9 +182,28 @@
 no github</t>
   </si>
   <si>
-    <t>Tela de forum onde
-os usuários do site
-poderam interagir entre si</t>
+    <t>Tela do quiz</t>
+  </si>
+  <si>
+    <t>Fazendo a conexão do banco de dados com o front-end</t>
+  </si>
+  <si>
+    <t>Integração com o banco de dados</t>
+  </si>
+  <si>
+    <t>SP1</t>
+  </si>
+  <si>
+    <t>SP2</t>
+  </si>
+  <si>
+    <t>SP3</t>
+  </si>
+  <si>
+    <t>SP4</t>
+  </si>
+  <si>
+    <t>TOTAL</t>
   </si>
 </sst>
 </file>
@@ -227,7 +234,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -252,8 +259,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -279,11 +292,26 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -295,14 +323,17 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -618,15 +649,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E0B76C4D-D953-4D8E-BEA3-2245CE848EF8}">
-  <dimension ref="A1:J15"/>
+  <dimension ref="A1:L15"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+      <selection activeCell="O3" sqref="O3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.7109375" customWidth="1"/>
+    <col min="1" max="1" width="34.85546875" customWidth="1"/>
     <col min="2" max="2" width="25.28515625" customWidth="1"/>
     <col min="3" max="3" width="18.140625" customWidth="1"/>
     <col min="4" max="4" width="18" customWidth="1"/>
@@ -635,21 +666,27 @@
     <col min="7" max="7" width="17" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A1" s="5" t="s">
+    <row r="1" spans="1:12" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5"/>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5"/>
-      <c r="F1" s="5"/>
-      <c r="G1" s="5"/>
-      <c r="H1" s="5"/>
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+      <c r="F1" s="7"/>
+      <c r="G1" s="7"/>
+      <c r="H1" s="7"/>
       <c r="I1" s="1"/>
       <c r="J1" s="3"/>
-    </row>
-    <row r="2" spans="1:10" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K1" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="L1" s="8">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>1</v>
       </c>
@@ -675,317 +712,367 @@
         <v>8</v>
       </c>
       <c r="I2" s="2"/>
-    </row>
-    <row r="3" spans="1:10" ht="60" x14ac:dyDescent="0.25">
-      <c r="A3" s="6" t="s">
+      <c r="K2" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="L2" s="8">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" ht="60" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="7" t="s">
+      <c r="B3" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="F3" s="5">
+        <v>8</v>
+      </c>
+      <c r="G3" s="5">
+        <v>5</v>
+      </c>
+      <c r="H3" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="K3" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="L3" s="8">
         <v>37</v>
       </c>
-      <c r="C3" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="D3" s="6" t="s">
+    </row>
+    <row r="4" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="D4" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="E3" s="6" t="s">
+      <c r="E4" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="F4" s="5">
+        <v>8</v>
+      </c>
+      <c r="G4" s="5">
+        <v>2</v>
+      </c>
+      <c r="H4" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="K4" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="L4" s="8">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" ht="75" x14ac:dyDescent="0.25">
+      <c r="A5" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="F5" s="5">
+        <v>8</v>
+      </c>
+      <c r="G5" s="5">
+        <v>1</v>
+      </c>
+      <c r="H5" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="K5" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="L5" s="8">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" ht="75" x14ac:dyDescent="0.25">
+      <c r="A6" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="E6" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="F3" s="6"/>
-      <c r="G3" s="6">
+      <c r="F6" s="5">
+        <v>21</v>
+      </c>
+      <c r="G6" s="5">
+        <v>6</v>
+      </c>
+      <c r="H6" s="5" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+      <c r="A7" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="F7" s="5">
         <v>5</v>
       </c>
-      <c r="H3" s="6" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="6" t="s">
+      <c r="G7" s="5">
+        <v>7</v>
+      </c>
+      <c r="H7" s="5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" ht="75" x14ac:dyDescent="0.25">
+      <c r="A8" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="F8" s="5">
+        <v>21</v>
+      </c>
+      <c r="G8" s="5">
+        <v>8</v>
+      </c>
+      <c r="H8" s="5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+      <c r="A9" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="E9" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="F9" s="5">
+        <v>21</v>
+      </c>
+      <c r="G9" s="5">
+        <v>3</v>
+      </c>
+      <c r="H9" s="5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+      <c r="A10" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="E10" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="F10" s="5">
+        <v>21</v>
+      </c>
+      <c r="G10" s="5">
+        <v>9</v>
+      </c>
+      <c r="H10" s="5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="A11" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="E11" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="F11" s="5">
+        <v>8</v>
+      </c>
+      <c r="G11" s="5">
         <v>10</v>
       </c>
-      <c r="B4" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="C4" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="D4" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="E4" s="6" t="s">
+      <c r="H11" s="5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="A12" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="E12" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="F12" s="5">
+        <v>3</v>
+      </c>
+      <c r="G12" s="5">
+        <v>4</v>
+      </c>
+      <c r="H12" s="5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="A13" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="E13" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="F4" s="6"/>
-      <c r="G4" s="6">
-        <v>2</v>
-      </c>
-      <c r="H4" s="6" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" ht="75" x14ac:dyDescent="0.25">
-      <c r="A5" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="B5" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="C5" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="D5" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="E5" s="6" t="s">
+      <c r="F13" s="5">
+        <v>21</v>
+      </c>
+      <c r="G13" s="5">
+        <v>12</v>
+      </c>
+      <c r="H13" s="5" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="B14" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="E14" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="F14" s="5">
+        <v>3</v>
+      </c>
+      <c r="G14" s="5">
+        <v>5</v>
+      </c>
+      <c r="H14" s="5" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+      <c r="A15" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="B15" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="D15" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="E15" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="F5" s="6"/>
-      <c r="G5" s="6">
-        <v>1</v>
-      </c>
-      <c r="H5" s="6" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" ht="75" x14ac:dyDescent="0.25">
-      <c r="A6" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="B6" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="C6" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="D6" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="E6" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="F6" s="6"/>
-      <c r="G6" s="6">
-        <v>6</v>
-      </c>
-      <c r="H6" s="6" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" ht="45" x14ac:dyDescent="0.25">
-      <c r="A7" s="6" t="s">
+      <c r="F15" s="5">
+        <v>21</v>
+      </c>
+      <c r="G15" s="5">
         <v>13</v>
       </c>
-      <c r="B7" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="C7" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="D7" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="E7" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="F7" s="6"/>
-      <c r="G7" s="6">
-        <v>7</v>
-      </c>
-      <c r="H7" s="6" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" ht="75" x14ac:dyDescent="0.25">
-      <c r="A8" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="B8" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="C8" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="D8" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="E8" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="F8" s="6"/>
-      <c r="G8" s="6">
-        <v>8</v>
-      </c>
-      <c r="H8" s="6" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" ht="45" x14ac:dyDescent="0.25">
-      <c r="A9" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="B9" s="7" t="s">
-        <v>43</v>
-      </c>
-      <c r="C9" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="D9" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="E9" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="F9" s="6"/>
-      <c r="G9" s="6">
-        <v>3</v>
-      </c>
-      <c r="H9" s="6" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" ht="45" x14ac:dyDescent="0.25">
-      <c r="A10" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="B10" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="C10" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="D10" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="E10" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="F10" s="6"/>
-      <c r="G10" s="6">
-        <v>9</v>
-      </c>
-      <c r="H10" s="6" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="A11" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="B11" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="C11" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="D11" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="E11" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="F11" s="6"/>
-      <c r="G11" s="6">
-        <v>10</v>
-      </c>
-      <c r="H11" s="6" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="A12" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="B12" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="C12" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="D12" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="E12" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="F12" s="6"/>
-      <c r="G12" s="6">
-        <v>4</v>
-      </c>
-      <c r="H12" s="6" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="A13" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="B13" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="C13" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="D13" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="E13" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="F13" s="6"/>
-      <c r="G13" s="6">
-        <v>12</v>
-      </c>
-      <c r="H13" s="6" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="B14" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="C14" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="D14" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="E14" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="F14" s="6"/>
-      <c r="G14" s="6">
-        <v>5</v>
-      </c>
-      <c r="H14" s="6" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" ht="45" x14ac:dyDescent="0.25">
-      <c r="A15" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="B15" s="7" t="s">
-        <v>49</v>
-      </c>
-      <c r="C15" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="D15" s="6" t="s">
+      <c r="H15" s="5" t="s">
         <v>32</v>
-      </c>
-      <c r="E15" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="F15" s="6"/>
-      <c r="G15" s="6">
-        <v>11</v>
-      </c>
-      <c r="H15" s="6" t="s">
-        <v>35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>